<commit_message>
more bits commented out (hopefully the last) 😊
</commit_message>
<xml_diff>
--- a/sw stats/ubuntu software stats.xlsx
+++ b/sw stats/ubuntu software stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Apt" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>Adobe Reader</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Quota</t>
+  </si>
+  <si>
+    <t>gdb</t>
   </si>
 </sst>
 </file>
@@ -710,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,6 +933,11 @@
       </c>
       <c r="E30" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>